<commit_message>
added emply list. added notes and fixed errors
</commit_message>
<xml_diff>
--- a/excel_sheets/Employees_Not_Set.xlsx
+++ b/excel_sheets/Employees_Not_Set.xlsx
@@ -482,7 +482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
@@ -548,7 +548,7 @@
           <t>Ben Berryhill</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n"/>
+      <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="5" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -569,8 +569,13 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="G2" s="5" t="n"/>
-      <c r="H2" s="3" t="n"/>
+      <c r="G2" s="5" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>hello there</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -1109,6 +1114,7 @@
         </is>
       </c>
     </row>
+    <row r="25"/>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
@@ -1484,11 +1490,6 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H15">

</xml_diff>